<commit_message>
Modification in AddNewProductFromExcel. working on protection against multiplet ElzabProductId
</commit_message>
<xml_diff>
--- a/Faktury i cenniki/ETS/Aktualizacja cen i vat 08.02.2021/Cennik hurtowy 12.2020.xlsx
+++ b/Faktury i cenniki/ETS/Aktualizacja cen i vat 08.02.2021/Cennik hurtowy 12.2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NaturalnieApp\NaturalnieApp\Faktury i cenniki\ETS\Aktualizacja cen i vat 08.02.2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E53CEA7-48DC-4F3D-BA33-FC0595D9EB8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4F51F5-1DB6-48A9-B562-A1ECC212A244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="3300" windowWidth="21495" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REGULAR" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="683">
   <si>
     <t>Zdjęcie</t>
   </si>
@@ -1357,106 +1357,766 @@
     <t>Ekologiczna herbatka ziołowa z cynamonem, rumiankiem, pokrzywą, koprem włoskim, burakiem, pomarańczą, czarną porzeczką i borówką. Składniki: ekologiczny cynamon (39%), ekologiczny rumianek (19%), ekologiczny koper włoski (13%), ekologiczny burak (12%), ekologiczna skórka pomarańczy (7%), ekologiczna pokrzywa (6%), ekologiczna czarna porzeczka (2%), ekologiczne borówki (2%).</t>
   </si>
   <si>
-    <t xml:space="preserve">SUPREME GREEN </t>
-  </si>
-  <si>
-    <t>THE GRATEST SIPS</t>
-  </si>
-  <si>
-    <t>BECAUSE YOU'RE AMAZING</t>
-  </si>
-  <si>
-    <t>GREEN TEA POMEGRANATE 15 SZT.</t>
-  </si>
-  <si>
-    <t>CHOCOLATE ROOIBOS &amp; VANILLA 15 SZT.</t>
-  </si>
-  <si>
-    <t>EARL GREY 15 SZT.</t>
-  </si>
-  <si>
-    <t>GREEN TEA 15 SZT.</t>
-  </si>
-  <si>
-    <t>ENGLISH BREAKFAST 15 SZT.</t>
-  </si>
-  <si>
-    <t>GINGER PEACH TEA 15 SZT.</t>
-  </si>
-  <si>
-    <t>SUPERBERRIES 15 SZT.</t>
-  </si>
-  <si>
-    <t>APPLE ROSEHIP RASPBERRY RIPPLE 15 SZT.</t>
-  </si>
-  <si>
-    <t>CHOCOLATE SUPER BERRY BURST 15 SZT.</t>
-  </si>
-  <si>
-    <t>PREMIUM ENGLISH BREAKFAST 50 CT</t>
-  </si>
-  <si>
-    <t>PREMIUM EARL GREY 50 CT</t>
-  </si>
-  <si>
-    <t>PREMIUM GREEN TEA &amp; POMEGRANATE 50CT</t>
-  </si>
-  <si>
-    <t>PREMIUM WHITE TEA COCONUT &amp; PASSION FRUIT 50 CT</t>
-  </si>
-  <si>
-    <t>PREMIUM SUPER BERRIES 50 CT</t>
-  </si>
-  <si>
-    <t>PREMIUM PURE GREEN TEA 50 CT</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ENGLISH BREAKFAST DOUBLE CHAMBER 100 SZT.</t>
-  </si>
-  <si>
-    <t>HERBATA BIO EARL GREY DOUBLE CHAMBER 100 SZT.</t>
-  </si>
-  <si>
-    <t>HERBATA BIO CLASSIC 12 PIRAMIDEK</t>
-  </si>
-  <si>
-    <t>HERBATA BIO  SUPER 12 PIRAMIDEK</t>
-  </si>
-  <si>
-    <t>HERBATA BIO WELLNESS 12 PIRAMIDEK</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW OKRĄGŁY 12 PIRAMIDEK</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW LUXURY 48 NEW</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW 48 CT EASTER PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HERBATA BIO ZESTAW 48 PINK COLOR </t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW 36 YOUR WELLNESS COLLECTION</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW 36 ULTIMATE TEA COLLECTION</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW 36 SUPER GOODNESS COLLECTION</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW LUXURY WHITE TIN 36 NEW</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW 72 ULTIMATE TEA COLLECTION</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW LUXURY 72 NEW</t>
-  </si>
-  <si>
-    <t>HERBATA BIO ZESTAW UNION JACK 72 NEW</t>
+    <t>Waga</t>
+  </si>
+  <si>
+    <t>2,5gx20</t>
+  </si>
+  <si>
+    <t>2,25gx20</t>
+  </si>
+  <si>
+    <t>2gx20</t>
+  </si>
+  <si>
+    <t>1.75gx20</t>
+  </si>
+  <si>
+    <t>1gx20</t>
+  </si>
+  <si>
+    <t>1,5gx20</t>
+  </si>
+  <si>
+    <t>1.5gx20</t>
+  </si>
+  <si>
+    <t>30g</t>
+  </si>
+  <si>
+    <t>3gx15</t>
+  </si>
+  <si>
+    <t>2.5gx15</t>
+  </si>
+  <si>
+    <t>2gx15x6</t>
+  </si>
+  <si>
+    <t>3gx50</t>
+  </si>
+  <si>
+    <t>2,5gx50</t>
+  </si>
+  <si>
+    <t>2gx50</t>
+  </si>
+  <si>
+    <t>80gx6</t>
+  </si>
+  <si>
+    <t>2,5gx100</t>
+  </si>
+  <si>
+    <t>2gx100</t>
+  </si>
+  <si>
+    <t>2gx12</t>
+  </si>
+  <si>
+    <t>English Breakfast 2,5gx20</t>
+  </si>
+  <si>
+    <t>Earl Grey  2,25gx20</t>
+  </si>
+  <si>
+    <t>Ceylon Black tea 2,25gx20</t>
+  </si>
+  <si>
+    <t>Darjeeling Black Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Decaffeinated Black Tea  2gx20</t>
+  </si>
+  <si>
+    <t>Vanilla Earl Grey 2gx20</t>
+  </si>
+  <si>
+    <t>Lemon Black Tea 1.75gx20</t>
+  </si>
+  <si>
+    <t>Mint Black Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Black Tea &amp; Ginger with Peach  2gx20</t>
+  </si>
+  <si>
+    <t>Chai Black Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Pure Green Tea  2gx20</t>
+  </si>
+  <si>
+    <t>Pure White Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Sencha Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Oolong Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Green Tea &amp; Pomegranate 2gx20</t>
+  </si>
+  <si>
+    <t>White Tea, Coconut &amp; Passion Fruit 2gx20</t>
+  </si>
+  <si>
+    <t>White Tea Lychee Cocoa 2gx20</t>
+  </si>
+  <si>
+    <t>Jasmine Green Tea 2gx20</t>
+  </si>
+  <si>
+    <t>Mint Green Tea 2gx20</t>
+  </si>
+  <si>
+    <t>White Tea Tropical Fruits 2gx20</t>
+  </si>
+  <si>
+    <t>Chamomile 1gx20</t>
+  </si>
+  <si>
+    <t>Perfect Peppermint 1,5gx20</t>
+  </si>
+  <si>
+    <t>Chamomile &amp; Lavender 1,5gx20</t>
+  </si>
+  <si>
+    <t>Chocolate, Rooibos &amp; Vanilla 2gx20</t>
+  </si>
+  <si>
+    <t>Lemongrass, Ginger &amp; Citrus 1,5gx20</t>
+  </si>
+  <si>
+    <t>Intense Chai 1.75gx20</t>
+  </si>
+  <si>
+    <t>Rooibos 2gx20</t>
+  </si>
+  <si>
+    <t>White Tea, Blueberry &amp; Elder Flower 2gx20</t>
+  </si>
+  <si>
+    <t>Super Berries 2gx20</t>
+  </si>
+  <si>
+    <t>Rooibos, Acai &amp; Pomegranate 1.5gx20</t>
+  </si>
+  <si>
+    <t>Apple, Rosehip &amp; Cinnamon 2gx20</t>
+  </si>
+  <si>
+    <t>Cranberry, Hibiscus &amp; Rosehip 1.75gx20</t>
+  </si>
+  <si>
+    <t>Green Rooibos, Pomegranate &amp; Blueberry 1.75gx20</t>
+  </si>
+  <si>
+    <t>Green Sencha, White Tea &amp; Matcha 1.75gx20</t>
+  </si>
+  <si>
+    <t>White Tea, Matcha &amp; Cinnamon 1.75gx20</t>
+  </si>
+  <si>
+    <t>Mighty Matcha 1.75gx20</t>
+  </si>
+  <si>
+    <t>Ceylon Cinnamon 1.75gx20</t>
+  </si>
+  <si>
+    <t>Mate, Cocoa &amp; Coconut 1.75gx20</t>
+  </si>
+  <si>
+    <t>Cocoa, Cinnamon &amp; Ginger 1.75gx20</t>
+  </si>
+  <si>
+    <t>Turmeric (Curcuma),  Ginger &amp; Lemongrass 1.75gx20</t>
+  </si>
+  <si>
+    <t>Cinamon, Moringa &amp; Ginger 1.75gx20</t>
+  </si>
+  <si>
+    <t>Beetroot, Apple &amp; Blueberry 1.5gx20</t>
+  </si>
+  <si>
+    <t>Beetroot, Ginger &amp; Curry Leaves 1.5gx20</t>
+  </si>
+  <si>
+    <t>Sleepy Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Shape Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Pure Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Happy Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Calm Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Energize Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Youthful Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Mama Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Beautiful Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Comfort Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>Revive Me 1.5gx20</t>
+  </si>
+  <si>
+    <t>MORNING, NOON &amp; NIGHTERS 39g</t>
+  </si>
+  <si>
+    <t>MOVERS &amp; SHAKERS 42g</t>
+  </si>
+  <si>
+    <t>TEAS FOR BUSY BEES 34g</t>
+  </si>
+  <si>
+    <t>SUPREME GREEN  37g</t>
+  </si>
+  <si>
+    <t>DAILY WELLNESS 30g</t>
+  </si>
+  <si>
+    <t>WOMAN’S WELLNESS 30g</t>
+  </si>
+  <si>
+    <t>A PURE SRI LANKAN 39g</t>
+  </si>
+  <si>
+    <t>LOVERLY MOTHERLY 34g</t>
+  </si>
+  <si>
+    <t>THE PERFECT GRADE 34g</t>
+  </si>
+  <si>
+    <t>THE GRATEST SIPS 34g</t>
+  </si>
+  <si>
+    <t>BECAUSE YOU'RE AMAZING 37g</t>
+  </si>
+  <si>
+    <t>English Breakfast 3gx15</t>
+  </si>
+  <si>
+    <t>Earl Grey 2.5gx15</t>
+  </si>
+  <si>
+    <t>Turmeric Ginger &amp; Lemongrass 2gx15x6</t>
+  </si>
+  <si>
+    <t>Lemon Black Tea 2gx15x6</t>
+  </si>
+  <si>
+    <t>Pure Green Tea 2gx15x6</t>
+  </si>
+  <si>
+    <t>Pure White Tea 2gx15x6</t>
+  </si>
+  <si>
+    <t>Green Tea &amp; Pomegranate 2gx15x6</t>
+  </si>
+  <si>
+    <t>White Tea, Coconut &amp; Passion 2gx15x6</t>
+  </si>
+  <si>
+    <t>Jasmine Green Tea 2gx15x6</t>
+  </si>
+  <si>
+    <t>White Tea, Blueberry &amp; Elder 2gx15x6</t>
+  </si>
+  <si>
+    <t>Super Berries 2gx15x6</t>
+  </si>
+  <si>
+    <t>Beetroot, Apple &amp; Blueberry 2gx15x6</t>
+  </si>
+  <si>
+    <t>Beetroot, Ginger &amp; Curry Lea 2gx15x6</t>
+  </si>
+  <si>
+    <t>Sleepy Me 2gx15x6</t>
+  </si>
+  <si>
+    <t>Beautiful Me 2gx15x6</t>
+  </si>
+  <si>
+    <t>Happy Me 2gx15x6</t>
+  </si>
+  <si>
+    <t>GREEN TEA POMEGRANATE 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>CHOCOLATE ROOIBOS &amp; VANILLA 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>EARL GREY 15 SZT. 2,5G*15</t>
+  </si>
+  <si>
+    <t>GREEN TEA 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>ENGLISH BREAKFAST 15 SZT. 3G*15</t>
+  </si>
+  <si>
+    <t>GINGER PEACH TEA 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>SUPERBERRIES 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>APPLE ROSEHIP RASPBERRY RIPPLE 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>CHOCOLATE SUPER BERRY BURST 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>WHITE TEA BLUEBERRY ELDERFLOWER 15 SZT. 2G*15</t>
+  </si>
+  <si>
+    <t>PREMIUM ENGLISH BREAKFAST 50 CT 3gx50</t>
+  </si>
+  <si>
+    <t>PREMIUM EARL GREY 50 CT 2,5gx50</t>
+  </si>
+  <si>
+    <t>PREMIUM GREEN TEA &amp; POMEGRANATE 50CT 2gx50</t>
+  </si>
+  <si>
+    <t>PREMIUM WHITE TEA COCONUT &amp; PASSION FRUIT 50 CT 2gx50</t>
+  </si>
+  <si>
+    <t>PREMIUM SUPER BERRIES 50 CT 2gx50</t>
+  </si>
+  <si>
+    <t>PREMIUM PURE GREEN TEA 50 CT 2gx50</t>
+  </si>
+  <si>
+    <t>English Breakfast 80gx6</t>
+  </si>
+  <si>
+    <t>Ceylon Black Tea 80gx6</t>
+  </si>
+  <si>
+    <t>Lemon Black lea 80gx6</t>
+  </si>
+  <si>
+    <t>Black Tea &amp; Ginger with Peach 80gx6</t>
+  </si>
+  <si>
+    <t>Pure White Tea 80gx6</t>
+  </si>
+  <si>
+    <t>Green Tea &amp;Pomegranate 80gx6</t>
+  </si>
+  <si>
+    <t>White Tea, Coconut &amp; Passion Fruit 80gx6</t>
+  </si>
+  <si>
+    <t>Jasmine Green Tea 80gx6</t>
+  </si>
+  <si>
+    <t>Perfect Peppermint 80gx6</t>
+  </si>
+  <si>
+    <t>Chocolate, Rooibos &amp; Vanilla 80gx6</t>
+  </si>
+  <si>
+    <t>Rooibos 80gx6</t>
+  </si>
+  <si>
+    <t>White Tea, Blueberry &amp;Elderflower 80gx6</t>
+  </si>
+  <si>
+    <t>Cranberry, Hibiscus &amp; Rosehip 80gx6</t>
+  </si>
+  <si>
+    <t>Turmeric (Curcuma), Ginger &amp; Lemongrass 80gx6</t>
+  </si>
+  <si>
+    <t>Pure Green Tea 80gx6</t>
+  </si>
+  <si>
+    <t>Earl Grey 80gx6</t>
+  </si>
+  <si>
+    <t>Super Berries 80gx6</t>
+  </si>
+  <si>
+    <t>Sleepy Me 80gx6</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ENGLISH BREAKFAST DOUBLE CHAMBER 100 SZT. 2,5gx100</t>
+  </si>
+  <si>
+    <t>HERBATA BIO EARL GREY DOUBLE CHAMBER 100 SZT. 2gx100</t>
+  </si>
+  <si>
+    <t>HERBATA BIO CLASSIC 12 PIRAMIDEK 2gx12</t>
+  </si>
+  <si>
+    <t>HERBATA BIO  SUPER 12 PIRAMIDEK 2gx12</t>
+  </si>
+  <si>
+    <t>HERBATA BIO WELLNESS 12 PIRAMIDEK 2gx12</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW OKRĄGŁY 12 PIRAMIDEK 2gx12</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW LUXURY 48 NEW 98g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW 48 CT EASTER PACK 72g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW 48 PINK COLOR  94g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW 36 YOUR WELLNESS COLLECTION 54g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW 36 ULTIMATE TEA COLLECTION 69g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW 36 SUPER GOODNESS COLLECTION 60g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW LUXURY WHITE TIN 36 NEW 73.5</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW 72 ULTIMATE TEA COLLECTION 136g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW LUXURY 72 NEW 136g</t>
+  </si>
+  <si>
+    <t>HERBATA BIO ZESTAW UNION JACK 72 NEW 136g</t>
+  </si>
+  <si>
+    <t>680275029090</t>
+  </si>
+  <si>
+    <t>680275029144</t>
+  </si>
+  <si>
+    <t>680275057857</t>
+  </si>
+  <si>
+    <t>680275040187</t>
+  </si>
+  <si>
+    <t>680275034469</t>
+  </si>
+  <si>
+    <t>680275057864</t>
+  </si>
+  <si>
+    <t>680275057765</t>
+  </si>
+  <si>
+    <t>680275057772</t>
+  </si>
+  <si>
+    <t>680275029212</t>
+  </si>
+  <si>
+    <t>680275029120</t>
+  </si>
+  <si>
+    <t>680275029151</t>
+  </si>
+  <si>
+    <t>680275029267</t>
+  </si>
+  <si>
+    <t>680275029182</t>
+  </si>
+  <si>
+    <t>680275057871</t>
+  </si>
+  <si>
+    <t>680275029083</t>
+  </si>
+  <si>
+    <t>680275052975</t>
+  </si>
+  <si>
+    <t>680275052999</t>
+  </si>
+  <si>
+    <t>680275057888</t>
+  </si>
+  <si>
+    <t>680275057895</t>
+  </si>
+  <si>
+    <t>680275057901</t>
+  </si>
+  <si>
+    <t>680275029250</t>
+  </si>
+  <si>
+    <t>680275029243</t>
+  </si>
+  <si>
+    <t>680275039419</t>
+  </si>
+  <si>
+    <t>680275029168</t>
+  </si>
+  <si>
+    <t>680275029137</t>
+  </si>
+  <si>
+    <t>680275057918</t>
+  </si>
+  <si>
+    <t>680275029106</t>
+  </si>
+  <si>
+    <t>680275039846</t>
+  </si>
+  <si>
+    <t>680275029236</t>
+  </si>
+  <si>
+    <t>680275057789</t>
+  </si>
+  <si>
+    <t>680275057925</t>
+  </si>
+  <si>
+    <t>680275057932</t>
+  </si>
+  <si>
+    <t>680275057987</t>
+  </si>
+  <si>
+    <t>680275057949</t>
+  </si>
+  <si>
+    <t>680275057796</t>
+  </si>
+  <si>
+    <t>680275057994</t>
+  </si>
+  <si>
+    <t>680275057185</t>
+  </si>
+  <si>
+    <t>680275057956</t>
+  </si>
+  <si>
+    <t>680275057239</t>
+  </si>
+  <si>
+    <t>680275057802</t>
+  </si>
+  <si>
+    <t>680275057192</t>
+  </si>
+  <si>
+    <t>680275057819</t>
+  </si>
+  <si>
+    <t>680275057826</t>
+  </si>
+  <si>
+    <t>680275043966</t>
+  </si>
+  <si>
+    <t>680275057970</t>
+  </si>
+  <si>
+    <t>680275057833</t>
+  </si>
+  <si>
+    <t>680275043935</t>
+  </si>
+  <si>
+    <t>680275057840</t>
+  </si>
+  <si>
+    <t>680275043928</t>
+  </si>
+  <si>
+    <t>680275043980</t>
+  </si>
+  <si>
+    <t>680275057253</t>
+  </si>
+  <si>
+    <t>680275057260</t>
+  </si>
+  <si>
+    <t>680275050728</t>
+  </si>
+  <si>
+    <t>680275048114</t>
+  </si>
+  <si>
+    <t>680275060390</t>
+  </si>
+  <si>
+    <t>680275060406</t>
+  </si>
+  <si>
+    <t>680275060413</t>
+  </si>
+  <si>
+    <t>680275060437</t>
+  </si>
+  <si>
+    <t>680275060420</t>
+  </si>
+  <si>
+    <t>680275060444</t>
+  </si>
+  <si>
+    <t>680275060161</t>
+  </si>
+  <si>
+    <t>680275060178</t>
+  </si>
+  <si>
+    <t>680275060154</t>
+  </si>
+  <si>
+    <t>680275060185</t>
+  </si>
+  <si>
+    <t>680275059455</t>
+  </si>
+  <si>
+    <t>680275059615</t>
+  </si>
+  <si>
+    <t>680275059493</t>
+  </si>
+  <si>
+    <t>680275059509</t>
+  </si>
+  <si>
+    <t>680275059516</t>
+  </si>
+  <si>
+    <t>680275059523</t>
+  </si>
+  <si>
+    <t>680275059530</t>
+  </si>
+  <si>
+    <t>680275059578</t>
+  </si>
+  <si>
+    <t>680275059585</t>
+  </si>
+  <si>
+    <t>680275059622</t>
+  </si>
+  <si>
+    <t>680275059660</t>
+  </si>
+  <si>
+    <t>680275059677</t>
+  </si>
+  <si>
+    <t>680275059707</t>
+  </si>
+  <si>
+    <t>680275059721</t>
+  </si>
+  <si>
+    <t>680275060055</t>
+  </si>
+  <si>
+    <t>680275059820</t>
+  </si>
+  <si>
+    <t>680275059844</t>
+  </si>
+  <si>
+    <t>680275059868</t>
+  </si>
+  <si>
+    <t>680275059889</t>
+  </si>
+  <si>
+    <t>680275059912</t>
+  </si>
+  <si>
+    <t>680275059929</t>
+  </si>
+  <si>
+    <t>680275059936</t>
+  </si>
+  <si>
+    <t>680275059967</t>
+  </si>
+  <si>
+    <t>680275059974</t>
+  </si>
+  <si>
+    <t>680275059998</t>
+  </si>
+  <si>
+    <t>680275060000</t>
+  </si>
+  <si>
+    <t>680275060024</t>
+  </si>
+  <si>
+    <t>680275060048</t>
+  </si>
+  <si>
+    <t>680275059882</t>
+  </si>
+  <si>
+    <t>680275059813</t>
+  </si>
+  <si>
+    <t>680275060017</t>
+  </si>
+  <si>
+    <t>680275059806</t>
+  </si>
+  <si>
+    <t>680275060864</t>
+  </si>
+  <si>
+    <t>680275060871</t>
+  </si>
+  <si>
+    <t>680275060888</t>
+  </si>
+  <si>
+    <t>680275060857</t>
+  </si>
+  <si>
+    <t>680275060826</t>
+  </si>
+  <si>
+    <t>680275058175</t>
+  </si>
+  <si>
+    <t>680275060833</t>
+  </si>
+  <si>
+    <t>680275060840</t>
   </si>
 </sst>
 </file>
@@ -1969,39 +2629,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2029,10 +2656,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9028,34 +9688,34 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="72"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="76"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="84"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="73"/>
     </row>
     <row r="4" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44">
@@ -10015,34 +10675,34 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="80"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="80"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="81"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="70"/>
     </row>
     <row r="34" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="78"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="67"/>
     </row>
     <row r="35" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
@@ -10177,19 +10837,19 @@
       </c>
     </row>
     <row r="39" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="85"/>
-      <c r="K39" s="86"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="78"/>
     </row>
     <row r="40" spans="1:11" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
@@ -10291,19 +10951,19 @@
       </c>
     </row>
     <row r="43" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="77"/>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="78"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="67"/>
     </row>
     <row r="44" spans="1:11" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
@@ -10471,19 +11131,19 @@
       </c>
     </row>
     <row r="49" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="76" t="s">
+      <c r="A49" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="77"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="77"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
-      <c r="I49" s="77"/>
-      <c r="J49" s="77"/>
-      <c r="K49" s="78"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="67"/>
     </row>
     <row r="50" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
@@ -10552,19 +11212,19 @@
       </c>
     </row>
     <row r="52" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="B52" s="77"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="77"/>
-      <c r="E52" s="77"/>
-      <c r="F52" s="77"/>
-      <c r="G52" s="77"/>
-      <c r="H52" s="77"/>
-      <c r="I52" s="77"/>
-      <c r="J52" s="77"/>
-      <c r="K52" s="78"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="66"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="67"/>
     </row>
     <row r="53" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -10928,19 +11588,19 @@
       </c>
     </row>
     <row r="64" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="68" t="s">
+      <c r="A64" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="69"/>
-      <c r="C64" s="69"/>
-      <c r="D64" s="69"/>
-      <c r="E64" s="69"/>
-      <c r="F64" s="69"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="69"/>
-      <c r="I64" s="69"/>
-      <c r="J64" s="69"/>
-      <c r="K64" s="70"/>
+      <c r="B64" s="82"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="82"/>
+      <c r="F64" s="82"/>
+      <c r="G64" s="82"/>
+      <c r="H64" s="82"/>
+      <c r="I64" s="82"/>
+      <c r="J64" s="82"/>
+      <c r="K64" s="83"/>
     </row>
     <row r="65" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
@@ -11180,19 +11840,19 @@
       </c>
     </row>
     <row r="72" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="68" t="s">
+      <c r="A72" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="B72" s="69"/>
-      <c r="C72" s="69"/>
-      <c r="D72" s="69"/>
-      <c r="E72" s="69"/>
-      <c r="F72" s="69"/>
-      <c r="G72" s="69"/>
-      <c r="H72" s="69"/>
-      <c r="I72" s="69"/>
-      <c r="J72" s="69"/>
-      <c r="K72" s="70"/>
+      <c r="B72" s="82"/>
+      <c r="C72" s="82"/>
+      <c r="D72" s="82"/>
+      <c r="E72" s="82"/>
+      <c r="F72" s="82"/>
+      <c r="G72" s="82"/>
+      <c r="H72" s="82"/>
+      <c r="I72" s="82"/>
+      <c r="J72" s="82"/>
+      <c r="K72" s="83"/>
     </row>
     <row r="73" spans="1:12" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16">
@@ -11337,19 +11997,19 @@
     </row>
     <row r="77" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="71" t="s">
+      <c r="A78" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="B78" s="67"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="67"/>
-      <c r="G78" s="67"/>
-      <c r="H78" s="67"/>
-      <c r="I78" s="67"/>
-      <c r="J78" s="67"/>
-      <c r="K78" s="72"/>
+      <c r="B78" s="75"/>
+      <c r="C78" s="75"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="75"/>
+      <c r="F78" s="75"/>
+      <c r="G78" s="75"/>
+      <c r="H78" s="75"/>
+      <c r="I78" s="75"/>
+      <c r="J78" s="75"/>
+      <c r="K78" s="76"/>
     </row>
     <row r="79" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="44">
@@ -11875,19 +12535,19 @@
       <c r="K95" s="33"/>
     </row>
     <row r="96" spans="1:11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="73" t="s">
+      <c r="A96" s="84" t="s">
         <v>207</v>
       </c>
-      <c r="B96" s="74"/>
-      <c r="C96" s="74"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="74"/>
-      <c r="G96" s="74"/>
-      <c r="H96" s="74"/>
-      <c r="I96" s="74"/>
-      <c r="J96" s="74"/>
-      <c r="K96" s="75"/>
+      <c r="B96" s="85"/>
+      <c r="C96" s="85"/>
+      <c r="D96" s="85"/>
+      <c r="E96" s="85"/>
+      <c r="F96" s="85"/>
+      <c r="G96" s="85"/>
+      <c r="H96" s="85"/>
+      <c r="I96" s="85"/>
+      <c r="J96" s="85"/>
+      <c r="K96" s="86"/>
     </row>
     <row r="97" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="16">
@@ -12219,19 +12879,19 @@
       <c r="K107" s="42"/>
     </row>
     <row r="108" spans="1:11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="73" t="s">
+      <c r="A108" s="84" t="s">
         <v>247</v>
       </c>
-      <c r="B108" s="74"/>
-      <c r="C108" s="74"/>
-      <c r="D108" s="74"/>
-      <c r="E108" s="74"/>
-      <c r="F108" s="74"/>
-      <c r="G108" s="74"/>
-      <c r="H108" s="74"/>
-      <c r="I108" s="74"/>
-      <c r="J108" s="74"/>
-      <c r="K108" s="75"/>
+      <c r="B108" s="85"/>
+      <c r="C108" s="85"/>
+      <c r="D108" s="85"/>
+      <c r="E108" s="85"/>
+      <c r="F108" s="85"/>
+      <c r="G108" s="85"/>
+      <c r="H108" s="85"/>
+      <c r="I108" s="85"/>
+      <c r="J108" s="85"/>
+      <c r="K108" s="86"/>
     </row>
     <row r="109" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="16">
@@ -12421,19 +13081,19 @@
     </row>
     <row r="115" spans="1:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="1:11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="73" t="s">
+      <c r="A116" s="84" t="s">
         <v>206</v>
       </c>
-      <c r="B116" s="74"/>
-      <c r="C116" s="74"/>
-      <c r="D116" s="74"/>
-      <c r="E116" s="74"/>
-      <c r="F116" s="74"/>
-      <c r="G116" s="74"/>
-      <c r="H116" s="74"/>
-      <c r="I116" s="74"/>
-      <c r="J116" s="74"/>
-      <c r="K116" s="75"/>
+      <c r="B116" s="85"/>
+      <c r="C116" s="85"/>
+      <c r="D116" s="85"/>
+      <c r="E116" s="85"/>
+      <c r="F116" s="85"/>
+      <c r="G116" s="85"/>
+      <c r="H116" s="85"/>
+      <c r="I116" s="85"/>
+      <c r="J116" s="85"/>
+      <c r="K116" s="86"/>
     </row>
     <row r="117" spans="1:11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="16">
@@ -12995,32 +13655,32 @@
     </row>
     <row r="135" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="1:11" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="66" t="s">
+      <c r="A136" s="80" t="s">
         <v>267</v>
       </c>
-      <c r="B136" s="67"/>
-      <c r="C136" s="67"/>
-      <c r="D136" s="67"/>
-      <c r="E136" s="67"/>
-      <c r="F136" s="67"/>
-      <c r="G136" s="67"/>
-      <c r="H136" s="67"/>
-      <c r="I136" s="67"/>
-      <c r="J136" s="67"/>
-      <c r="K136" s="67"/>
+      <c r="B136" s="75"/>
+      <c r="C136" s="75"/>
+      <c r="D136" s="75"/>
+      <c r="E136" s="75"/>
+      <c r="F136" s="75"/>
+      <c r="G136" s="75"/>
+      <c r="H136" s="75"/>
+      <c r="I136" s="75"/>
+      <c r="J136" s="75"/>
+      <c r="K136" s="75"/>
     </row>
     <row r="137" spans="1:11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="65"/>
-      <c r="B137" s="65"/>
-      <c r="C137" s="65"/>
-      <c r="D137" s="65"/>
-      <c r="E137" s="65"/>
-      <c r="F137" s="65"/>
-      <c r="G137" s="65"/>
-      <c r="H137" s="65"/>
-      <c r="I137" s="65"/>
-      <c r="J137" s="65"/>
-      <c r="K137" s="65"/>
+      <c r="A137" s="79"/>
+      <c r="B137" s="79"/>
+      <c r="C137" s="79"/>
+      <c r="D137" s="79"/>
+      <c r="E137" s="79"/>
+      <c r="F137" s="79"/>
+      <c r="G137" s="79"/>
+      <c r="H137" s="79"/>
+      <c r="I137" s="79"/>
+      <c r="J137" s="79"/>
+      <c r="K137" s="79"/>
     </row>
     <row r="138" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="8">
@@ -13684,6 +14344,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A137:K137"/>
+    <mergeCell ref="A136:K136"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A72:K72"/>
+    <mergeCell ref="A78:K78"/>
+    <mergeCell ref="A116:K116"/>
+    <mergeCell ref="A96:K96"/>
+    <mergeCell ref="A108:K108"/>
     <mergeCell ref="A52:K52"/>
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="A3:K3"/>
@@ -13692,14 +14360,6 @@
     <mergeCell ref="A39:K39"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A137:K137"/>
-    <mergeCell ref="A136:K136"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A72:K72"/>
-    <mergeCell ref="A78:K78"/>
-    <mergeCell ref="A116:K116"/>
-    <mergeCell ref="A96:K96"/>
-    <mergeCell ref="A108:K108"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13712,8 +14372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2372160D-0FDE-4020-B4F7-7A907DA2382D}">
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13721,7 +14381,7 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.85546875" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -13744,7 +14404,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>429</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -13767,7 +14427,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>448</v>
       </c>
       <c r="D2" t="s">
         <v>356</v>
@@ -13776,7 +14436,7 @@
         <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>430</v>
       </c>
       <c r="G2">
         <v>8.94</v>
@@ -13784,8 +14444,8 @@
       <c r="H2">
         <v>16.899999999999999</v>
       </c>
-      <c r="I2">
-        <v>680275029090</v>
+      <c r="I2" t="s">
+        <v>579</v>
       </c>
       <c r="J2">
         <v>0.23</v>
@@ -13799,7 +14459,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="D3" t="s">
         <v>359</v>
@@ -13808,7 +14468,7 @@
         <v>132</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>431</v>
       </c>
       <c r="G3">
         <v>8.94</v>
@@ -13816,8 +14476,8 @@
       <c r="H3">
         <v>16.899999999999999</v>
       </c>
-      <c r="I3">
-        <v>680275029144</v>
+      <c r="I3" t="s">
+        <v>580</v>
       </c>
       <c r="J3">
         <v>0.23</v>
@@ -13831,7 +14491,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>450</v>
       </c>
       <c r="D4" t="s">
         <v>333</v>
@@ -13840,7 +14500,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>431</v>
       </c>
       <c r="G4">
         <v>8.94</v>
@@ -13848,8 +14508,8 @@
       <c r="H4">
         <v>16.899999999999999</v>
       </c>
-      <c r="I4">
-        <v>680275057857</v>
+      <c r="I4" t="s">
+        <v>581</v>
       </c>
       <c r="J4">
         <v>0.23</v>
@@ -13863,7 +14523,7 @@
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>451</v>
       </c>
       <c r="D5" t="s">
         <v>357</v>
@@ -13872,7 +14532,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G5">
         <v>8.94</v>
@@ -13880,8 +14540,8 @@
       <c r="H5">
         <v>16.899999999999999</v>
       </c>
-      <c r="I5">
-        <v>680275040187</v>
+      <c r="I5" t="s">
+        <v>582</v>
       </c>
       <c r="J5">
         <v>0.23</v>
@@ -13895,7 +14555,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>452</v>
       </c>
       <c r="D6" t="s">
         <v>334</v>
@@ -13904,7 +14564,7 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G6">
         <v>8.94</v>
@@ -13912,8 +14572,8 @@
       <c r="H6">
         <v>16.899999999999999</v>
       </c>
-      <c r="I6">
-        <v>680275034469</v>
+      <c r="I6" t="s">
+        <v>583</v>
       </c>
       <c r="J6">
         <v>0.23</v>
@@ -13927,7 +14587,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>453</v>
       </c>
       <c r="D7" t="s">
         <v>360</v>
@@ -13936,7 +14596,7 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G7">
         <v>8.94</v>
@@ -13944,8 +14604,8 @@
       <c r="H7">
         <v>16.899999999999999</v>
       </c>
-      <c r="I7">
-        <v>680275057864</v>
+      <c r="I7" t="s">
+        <v>584</v>
       </c>
       <c r="J7">
         <v>0.23</v>
@@ -13959,7 +14619,7 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>454</v>
       </c>
       <c r="D8" t="s">
         <v>335</v>
@@ -13968,7 +14628,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G8">
         <v>8.94</v>
@@ -13976,8 +14636,8 @@
       <c r="H8">
         <v>16.899999999999999</v>
       </c>
-      <c r="I8">
-        <v>680275057765</v>
+      <c r="I8" t="s">
+        <v>585</v>
       </c>
       <c r="J8">
         <v>0.23</v>
@@ -13991,7 +14651,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="D9" t="s">
         <v>419</v>
@@ -14000,7 +14660,7 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G9">
         <v>8.94</v>
@@ -14008,8 +14668,8 @@
       <c r="H9">
         <v>16.899999999999999</v>
       </c>
-      <c r="I9">
-        <v>680275057772</v>
+      <c r="I9" t="s">
+        <v>586</v>
       </c>
       <c r="J9">
         <v>0.23</v>
@@ -14023,7 +14683,7 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>456</v>
       </c>
       <c r="D10" t="s">
         <v>345</v>
@@ -14032,7 +14692,7 @@
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G10">
         <v>8.94</v>
@@ -14040,8 +14700,8 @@
       <c r="H10">
         <v>16.899999999999999</v>
       </c>
-      <c r="I10">
-        <v>680275029212</v>
+      <c r="I10" t="s">
+        <v>587</v>
       </c>
       <c r="J10">
         <v>0.23</v>
@@ -14055,7 +14715,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>457</v>
       </c>
       <c r="D11" t="s">
         <v>346</v>
@@ -14064,7 +14724,7 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G11">
         <v>8.94</v>
@@ -14072,8 +14732,8 @@
       <c r="H11">
         <v>16.899999999999999</v>
       </c>
-      <c r="I11">
-        <v>680275029120</v>
+      <c r="I11" t="s">
+        <v>588</v>
       </c>
       <c r="J11">
         <v>0.23</v>
@@ -14087,7 +14747,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>458</v>
       </c>
       <c r="D12" t="s">
         <v>362</v>
@@ -14096,7 +14756,7 @@
         <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G12">
         <v>8.94</v>
@@ -14104,8 +14764,8 @@
       <c r="H12">
         <v>16.899999999999999</v>
       </c>
-      <c r="I12">
-        <v>680275029151</v>
+      <c r="I12" t="s">
+        <v>589</v>
       </c>
       <c r="J12">
         <v>0.23</v>
@@ -14119,7 +14779,7 @@
         <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>459</v>
       </c>
       <c r="D13" t="s">
         <v>358</v>
@@ -14128,7 +14788,7 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G13">
         <v>8.94</v>
@@ -14136,8 +14796,8 @@
       <c r="H13">
         <v>16.899999999999999</v>
       </c>
-      <c r="I13">
-        <v>680275029267</v>
+      <c r="I13" t="s">
+        <v>590</v>
       </c>
       <c r="J13">
         <v>0.23</v>
@@ -14151,7 +14811,7 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>460</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -14160,7 +14820,7 @@
         <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G14">
         <v>8.94</v>
@@ -14168,8 +14828,8 @@
       <c r="H14">
         <v>16.899999999999999</v>
       </c>
-      <c r="I14">
-        <v>680275029182</v>
+      <c r="I14" t="s">
+        <v>591</v>
       </c>
       <c r="J14">
         <v>0.23</v>
@@ -14183,7 +14843,7 @@
         <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>461</v>
       </c>
       <c r="D15" t="s">
         <v>361</v>
@@ -14192,7 +14852,7 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G15">
         <v>8.94</v>
@@ -14200,8 +14860,8 @@
       <c r="H15">
         <v>16.899999999999999</v>
       </c>
-      <c r="I15">
-        <v>680275057871</v>
+      <c r="I15" t="s">
+        <v>592</v>
       </c>
       <c r="J15">
         <v>0.23</v>
@@ -14215,7 +14875,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>462</v>
       </c>
       <c r="D16" t="s">
         <v>363</v>
@@ -14224,7 +14884,7 @@
         <v>132</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G16">
         <v>8.94</v>
@@ -14232,8 +14892,8 @@
       <c r="H16">
         <v>16.899999999999999</v>
       </c>
-      <c r="I16">
-        <v>680275029083</v>
+      <c r="I16" t="s">
+        <v>593</v>
       </c>
       <c r="J16">
         <v>0.23</v>
@@ -14247,7 +14907,7 @@
         <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>463</v>
       </c>
       <c r="D17" t="s">
         <v>364</v>
@@ -14256,7 +14916,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G17">
         <v>8.94</v>
@@ -14264,8 +14924,8 @@
       <c r="H17">
         <v>16.899999999999999</v>
       </c>
-      <c r="I17">
-        <v>680275052975</v>
+      <c r="I17" t="s">
+        <v>594</v>
       </c>
       <c r="J17">
         <v>0.23</v>
@@ -14279,7 +14939,7 @@
         <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>464</v>
       </c>
       <c r="D18" t="s">
         <v>337</v>
@@ -14288,7 +14948,7 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G18">
         <v>8.94</v>
@@ -14296,8 +14956,8 @@
       <c r="H18">
         <v>16.899999999999999</v>
       </c>
-      <c r="I18">
-        <v>680275052999</v>
+      <c r="I18" t="s">
+        <v>595</v>
       </c>
       <c r="J18">
         <v>0.23</v>
@@ -14311,7 +14971,7 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>465</v>
       </c>
       <c r="D19" t="s">
         <v>365</v>
@@ -14320,7 +14980,7 @@
         <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G19">
         <v>8.94</v>
@@ -14328,8 +14988,8 @@
       <c r="H19">
         <v>16.899999999999999</v>
       </c>
-      <c r="I19">
-        <v>680275057888</v>
+      <c r="I19" t="s">
+        <v>596</v>
       </c>
       <c r="J19">
         <v>0.23</v>
@@ -14343,7 +15003,7 @@
         <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>466</v>
       </c>
       <c r="D20" t="s">
         <v>338</v>
@@ -14352,7 +15012,7 @@
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G20">
         <v>8.94</v>
@@ -14360,8 +15020,8 @@
       <c r="H20">
         <v>16.899999999999999</v>
       </c>
-      <c r="I20">
-        <v>680275057895</v>
+      <c r="I20" t="s">
+        <v>597</v>
       </c>
       <c r="J20">
         <v>0.23</v>
@@ -14375,7 +15035,7 @@
         <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>467</v>
       </c>
       <c r="D21" t="s">
         <v>366</v>
@@ -14384,7 +15044,7 @@
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G21">
         <v>8.94</v>
@@ -14392,8 +15052,8 @@
       <c r="H21">
         <v>16.899999999999999</v>
       </c>
-      <c r="I21">
-        <v>680275057901</v>
+      <c r="I21" t="s">
+        <v>598</v>
       </c>
       <c r="J21">
         <v>0.23</v>
@@ -14407,7 +15067,7 @@
         <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>468</v>
       </c>
       <c r="D22" t="s">
         <v>367</v>
@@ -14416,7 +15076,7 @@
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>434</v>
       </c>
       <c r="G22">
         <v>8.94</v>
@@ -14424,8 +15084,8 @@
       <c r="H22">
         <v>16.899999999999999</v>
       </c>
-      <c r="I22">
-        <v>680275029250</v>
+      <c r="I22" t="s">
+        <v>599</v>
       </c>
       <c r="J22">
         <v>0.23</v>
@@ -14439,7 +15099,7 @@
         <v>112</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>469</v>
       </c>
       <c r="D23" t="s">
         <v>420</v>
@@ -14448,7 +15108,7 @@
         <v>132</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>435</v>
       </c>
       <c r="G23">
         <v>8.94</v>
@@ -14456,8 +15116,8 @@
       <c r="H23">
         <v>16.899999999999999</v>
       </c>
-      <c r="I23">
-        <v>680275029243</v>
+      <c r="I23" t="s">
+        <v>600</v>
       </c>
       <c r="J23">
         <v>0.08</v>
@@ -14471,7 +15131,7 @@
         <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>470</v>
       </c>
       <c r="D24" t="s">
         <v>368</v>
@@ -14480,7 +15140,7 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>435</v>
       </c>
       <c r="G24">
         <v>8.94</v>
@@ -14488,8 +15148,8 @@
       <c r="H24">
         <v>16.899999999999999</v>
       </c>
-      <c r="I24">
-        <v>680275039419</v>
+      <c r="I24" t="s">
+        <v>601</v>
       </c>
       <c r="J24">
         <v>0.08</v>
@@ -14503,7 +15163,7 @@
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>471</v>
       </c>
       <c r="D25" t="s">
         <v>347</v>
@@ -14512,7 +15172,7 @@
         <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G25">
         <v>8.94</v>
@@ -14520,8 +15180,8 @@
       <c r="H25">
         <v>16.899999999999999</v>
       </c>
-      <c r="I25">
-        <v>680275029168</v>
+      <c r="I25" t="s">
+        <v>602</v>
       </c>
       <c r="J25">
         <v>0.23</v>
@@ -14535,7 +15195,7 @@
         <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>472</v>
       </c>
       <c r="D26" t="s">
         <v>421</v>
@@ -14544,7 +15204,7 @@
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>117</v>
+        <v>435</v>
       </c>
       <c r="G26">
         <v>8.94</v>
@@ -14552,8 +15212,8 @@
       <c r="H26">
         <v>16.899999999999999</v>
       </c>
-      <c r="I26">
-        <v>680275029137</v>
+      <c r="I26" t="s">
+        <v>603</v>
       </c>
       <c r="J26">
         <v>0.08</v>
@@ -14567,7 +15227,7 @@
         <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>473</v>
       </c>
       <c r="D27" t="s">
         <v>422</v>
@@ -14576,7 +15236,7 @@
         <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G27">
         <v>8.94</v>
@@ -14584,8 +15244,8 @@
       <c r="H27">
         <v>16.899999999999999</v>
       </c>
-      <c r="I27">
-        <v>680275057918</v>
+      <c r="I27" t="s">
+        <v>604</v>
       </c>
       <c r="J27">
         <v>0.08</v>
@@ -14599,7 +15259,7 @@
         <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>474</v>
       </c>
       <c r="D28" t="s">
         <v>369</v>
@@ -14608,7 +15268,7 @@
         <v>132</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G28">
         <v>8.94</v>
@@ -14616,8 +15276,8 @@
       <c r="H28">
         <v>16.899999999999999</v>
       </c>
-      <c r="I28">
-        <v>680275029106</v>
+      <c r="I28" t="s">
+        <v>605</v>
       </c>
       <c r="J28">
         <v>0.08</v>
@@ -14631,7 +15291,7 @@
         <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>475</v>
       </c>
       <c r="D29" t="s">
         <v>370</v>
@@ -14640,7 +15300,7 @@
         <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G29">
         <v>8.94</v>
@@ -14648,8 +15308,8 @@
       <c r="H29">
         <v>16.899999999999999</v>
       </c>
-      <c r="I29">
-        <v>680275039846</v>
+      <c r="I29" t="s">
+        <v>606</v>
       </c>
       <c r="J29">
         <v>0.23</v>
@@ -14663,7 +15323,7 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>476</v>
       </c>
       <c r="D30" t="s">
         <v>371</v>
@@ -14672,7 +15332,7 @@
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G30">
         <v>8.94</v>
@@ -14680,8 +15340,8 @@
       <c r="H30">
         <v>16.899999999999999</v>
       </c>
-      <c r="I30">
-        <v>680275029236</v>
+      <c r="I30" t="s">
+        <v>607</v>
       </c>
       <c r="J30">
         <v>0.08</v>
@@ -14695,7 +15355,7 @@
         <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>477</v>
       </c>
       <c r="D31" t="s">
         <v>372</v>
@@ -14704,7 +15364,7 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G31">
         <v>8.94</v>
@@ -14712,8 +15372,8 @@
       <c r="H31">
         <v>16.899999999999999</v>
       </c>
-      <c r="I31">
-        <v>680275057789</v>
+      <c r="I31" t="s">
+        <v>608</v>
       </c>
       <c r="J31">
         <v>0.08</v>
@@ -14727,7 +15387,7 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>478</v>
       </c>
       <c r="D32" t="s">
         <v>348</v>
@@ -14736,7 +15396,7 @@
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="G32">
         <v>8.94</v>
@@ -14744,8 +15404,8 @@
       <c r="H32">
         <v>16.899999999999999</v>
       </c>
-      <c r="I32">
-        <v>680275057925</v>
+      <c r="I32" t="s">
+        <v>609</v>
       </c>
       <c r="J32">
         <v>0.08</v>
@@ -14759,7 +15419,7 @@
         <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>479</v>
       </c>
       <c r="D33" t="s">
         <v>349</v>
@@ -14768,7 +15428,7 @@
         <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G33">
         <v>8.94</v>
@@ -14776,8 +15436,8 @@
       <c r="H33">
         <v>16.899999999999999</v>
       </c>
-      <c r="I33">
-        <v>680275057932</v>
+      <c r="I33" t="s">
+        <v>610</v>
       </c>
       <c r="J33">
         <v>0.08</v>
@@ -14791,7 +15451,7 @@
         <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>480</v>
       </c>
       <c r="D34" t="s">
         <v>373</v>
@@ -14800,7 +15460,7 @@
         <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G34">
         <v>8.94</v>
@@ -14808,8 +15468,8 @@
       <c r="H34">
         <v>16.899999999999999</v>
       </c>
-      <c r="I34">
-        <v>680275057987</v>
+      <c r="I34" t="s">
+        <v>611</v>
       </c>
       <c r="J34">
         <v>0.08</v>
@@ -14823,7 +15483,7 @@
         <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>481</v>
       </c>
       <c r="D35" t="s">
         <v>339</v>
@@ -14832,7 +15492,7 @@
         <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G35">
         <v>8.94</v>
@@ -14840,8 +15500,8 @@
       <c r="H35">
         <v>16.899999999999999</v>
       </c>
-      <c r="I35">
-        <v>680275057949</v>
+      <c r="I35" t="s">
+        <v>612</v>
       </c>
       <c r="J35">
         <v>0.23</v>
@@ -14855,7 +15515,7 @@
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>482</v>
       </c>
       <c r="D36" t="s">
         <v>374</v>
@@ -14864,7 +15524,7 @@
         <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G36">
         <v>8.94</v>
@@ -14872,8 +15532,8 @@
       <c r="H36">
         <v>16.899999999999999</v>
       </c>
-      <c r="I36">
-        <v>680275057796</v>
+      <c r="I36" t="s">
+        <v>613</v>
       </c>
       <c r="J36">
         <v>0.23</v>
@@ -14887,7 +15547,7 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>483</v>
       </c>
       <c r="D37" t="s">
         <v>375</v>
@@ -14896,7 +15556,7 @@
         <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G37">
         <v>8.94</v>
@@ -14904,8 +15564,8 @@
       <c r="H37">
         <v>16.899999999999999</v>
       </c>
-      <c r="I37">
-        <v>680275057994</v>
+      <c r="I37" t="s">
+        <v>614</v>
       </c>
       <c r="J37">
         <v>0.23</v>
@@ -14919,7 +15579,7 @@
         <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>484</v>
       </c>
       <c r="D38" t="s">
         <v>423</v>
@@ -14928,7 +15588,7 @@
         <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G38">
         <v>8.94</v>
@@ -14936,8 +15596,8 @@
       <c r="H38">
         <v>16.899999999999999</v>
       </c>
-      <c r="I38">
-        <v>680275057185</v>
+      <c r="I38" t="s">
+        <v>615</v>
       </c>
       <c r="J38">
         <v>0.23</v>
@@ -14951,7 +15611,7 @@
         <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>485</v>
       </c>
       <c r="D39" t="s">
         <v>424</v>
@@ -14960,7 +15620,7 @@
         <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G39">
         <v>8.94</v>
@@ -14968,8 +15628,8 @@
       <c r="H39">
         <v>16.899999999999999</v>
       </c>
-      <c r="I39">
-        <v>680275057956</v>
+      <c r="I39" t="s">
+        <v>616</v>
       </c>
       <c r="J39">
         <v>0.23</v>
@@ -14983,7 +15643,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>486</v>
       </c>
       <c r="D40" t="s">
         <v>425</v>
@@ -14992,7 +15652,7 @@
         <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G40">
         <v>8.94</v>
@@ -15000,8 +15660,8 @@
       <c r="H40">
         <v>16.899999999999999</v>
       </c>
-      <c r="I40">
-        <v>680275057239</v>
+      <c r="I40" t="s">
+        <v>617</v>
       </c>
       <c r="J40">
         <v>0.23</v>
@@ -15015,7 +15675,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>63</v>
+        <v>487</v>
       </c>
       <c r="D41" t="s">
         <v>376</v>
@@ -15024,7 +15684,7 @@
         <v>16</v>
       </c>
       <c r="F41" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G41">
         <v>8.94</v>
@@ -15032,8 +15692,8 @@
       <c r="H41">
         <v>16.899999999999999</v>
       </c>
-      <c r="I41">
-        <v>680275057802</v>
+      <c r="I41" t="s">
+        <v>618</v>
       </c>
       <c r="J41">
         <v>0.08</v>
@@ -15047,7 +15707,7 @@
         <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>488</v>
       </c>
       <c r="D42" t="s">
         <v>426</v>
@@ -15056,7 +15716,7 @@
         <v>16</v>
       </c>
       <c r="F42" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="G42">
         <v>8.94</v>
@@ -15064,8 +15724,8 @@
       <c r="H42">
         <v>16.899999999999999</v>
       </c>
-      <c r="I42">
-        <v>680275057192</v>
+      <c r="I42" t="s">
+        <v>619</v>
       </c>
       <c r="J42">
         <v>0.08</v>
@@ -15079,7 +15739,7 @@
         <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>489</v>
       </c>
       <c r="D43" t="s">
         <v>427</v>
@@ -15088,7 +15748,7 @@
         <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G43">
         <v>8.94</v>
@@ -15096,8 +15756,8 @@
       <c r="H43">
         <v>16.899999999999999</v>
       </c>
-      <c r="I43">
-        <v>680275057819</v>
+      <c r="I43" t="s">
+        <v>620</v>
       </c>
       <c r="J43">
         <v>0.08</v>
@@ -15111,7 +15771,7 @@
         <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>490</v>
       </c>
       <c r="D44" t="s">
         <v>350</v>
@@ -15120,7 +15780,7 @@
         <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G44">
         <v>8.94</v>
@@ -15128,8 +15788,8 @@
       <c r="H44">
         <v>16.899999999999999</v>
       </c>
-      <c r="I44">
-        <v>680275057826</v>
+      <c r="I44" t="s">
+        <v>621</v>
       </c>
       <c r="J44">
         <v>0.08</v>
@@ -15143,7 +15803,7 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>491</v>
       </c>
       <c r="D45" t="s">
         <v>377</v>
@@ -15152,7 +15812,7 @@
         <v>16</v>
       </c>
       <c r="F45" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G45">
         <v>8.94</v>
@@ -15160,8 +15820,8 @@
       <c r="H45">
         <v>14.9</v>
       </c>
-      <c r="I45">
-        <v>680275043966</v>
+      <c r="I45" t="s">
+        <v>622</v>
       </c>
       <c r="J45">
         <v>0.08</v>
@@ -15175,7 +15835,7 @@
         <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>492</v>
       </c>
       <c r="D46" t="s">
         <v>340</v>
@@ -15184,7 +15844,7 @@
         <v>16</v>
       </c>
       <c r="F46" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G46">
         <v>8.94</v>
@@ -15192,8 +15852,8 @@
       <c r="H46">
         <v>14.9</v>
       </c>
-      <c r="I46">
-        <v>680275057970</v>
+      <c r="I46" t="s">
+        <v>623</v>
       </c>
       <c r="J46">
         <v>0.23</v>
@@ -15207,7 +15867,7 @@
         <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>493</v>
       </c>
       <c r="D47" t="s">
         <v>351</v>
@@ -15216,7 +15876,7 @@
         <v>16</v>
       </c>
       <c r="F47" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G47">
         <v>8.94</v>
@@ -15224,8 +15884,8 @@
       <c r="H47">
         <v>14.9</v>
       </c>
-      <c r="I47">
-        <v>680275057833</v>
+      <c r="I47" t="s">
+        <v>624</v>
       </c>
       <c r="J47">
         <v>0.08</v>
@@ -15239,7 +15899,7 @@
         <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>494</v>
       </c>
       <c r="D48" t="s">
         <v>352</v>
@@ -15248,7 +15908,7 @@
         <v>16</v>
       </c>
       <c r="F48" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G48">
         <v>8.94</v>
@@ -15256,8 +15916,8 @@
       <c r="H48">
         <v>14.9</v>
       </c>
-      <c r="I48">
-        <v>680275043935</v>
+      <c r="I48" t="s">
+        <v>625</v>
       </c>
       <c r="J48">
         <v>0.08</v>
@@ -15271,7 +15931,7 @@
         <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>495</v>
       </c>
       <c r="D49" t="s">
         <v>353</v>
@@ -15280,7 +15940,7 @@
         <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G49">
         <v>8.94</v>
@@ -15288,8 +15948,8 @@
       <c r="H49">
         <v>14.9</v>
       </c>
-      <c r="I49">
-        <v>680275057840</v>
+      <c r="I49" t="s">
+        <v>626</v>
       </c>
       <c r="J49">
         <v>0.08</v>
@@ -15303,7 +15963,7 @@
         <v>78</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>496</v>
       </c>
       <c r="D50" t="s">
         <v>378</v>
@@ -15312,7 +15972,7 @@
         <v>16</v>
       </c>
       <c r="F50" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G50">
         <v>8.94</v>
@@ -15320,8 +15980,8 @@
       <c r="H50">
         <v>14.9</v>
       </c>
-      <c r="I50">
-        <v>680275043928</v>
+      <c r="I50" t="s">
+        <v>627</v>
       </c>
       <c r="J50">
         <v>0.08</v>
@@ -15335,7 +15995,7 @@
         <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>497</v>
       </c>
       <c r="D51" t="s">
         <v>341</v>
@@ -15344,7 +16004,7 @@
         <v>16</v>
       </c>
       <c r="F51" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G51">
         <v>8.94</v>
@@ -15352,8 +16012,8 @@
       <c r="H51">
         <v>14.9</v>
       </c>
-      <c r="I51">
-        <v>680275043980</v>
+      <c r="I51" t="s">
+        <v>628</v>
       </c>
       <c r="J51">
         <v>0.08</v>
@@ -15367,7 +16027,7 @@
         <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>498</v>
       </c>
       <c r="D52" t="s">
         <v>428</v>
@@ -15376,7 +16036,7 @@
         <v>16</v>
       </c>
       <c r="F52" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G52">
         <v>8.94</v>
@@ -15384,8 +16044,8 @@
       <c r="H52">
         <v>14.9</v>
       </c>
-      <c r="I52">
-        <v>680275057253</v>
+      <c r="I52" t="s">
+        <v>629</v>
       </c>
       <c r="J52">
         <v>0.08</v>
@@ -15399,7 +16059,7 @@
         <v>84</v>
       </c>
       <c r="C53" t="s">
-        <v>85</v>
+        <v>499</v>
       </c>
       <c r="D53" t="s">
         <v>354</v>
@@ -15408,7 +16068,7 @@
         <v>16</v>
       </c>
       <c r="F53" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G53">
         <v>8.94</v>
@@ -15416,8 +16076,8 @@
       <c r="H53">
         <v>14.9</v>
       </c>
-      <c r="I53">
-        <v>680275057260</v>
+      <c r="I53" t="s">
+        <v>630</v>
       </c>
       <c r="J53">
         <v>0.08</v>
@@ -15431,7 +16091,7 @@
         <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>500</v>
       </c>
       <c r="D54" t="s">
         <v>355</v>
@@ -15440,7 +16100,7 @@
         <v>16</v>
       </c>
       <c r="F54" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G54">
         <v>8.94</v>
@@ -15448,8 +16108,8 @@
       <c r="H54">
         <v>14.9</v>
       </c>
-      <c r="I54">
-        <v>680275050728</v>
+      <c r="I54" t="s">
+        <v>631</v>
       </c>
       <c r="J54">
         <v>0.08</v>
@@ -15463,13 +16123,13 @@
         <v>88</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>501</v>
       </c>
       <c r="E55" t="s">
         <v>16</v>
       </c>
       <c r="F55" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="G55">
         <v>8.94</v>
@@ -15477,8 +16137,8 @@
       <c r="H55">
         <v>14.9</v>
       </c>
-      <c r="I55">
-        <v>680275048114</v>
+      <c r="I55" t="s">
+        <v>632</v>
       </c>
       <c r="J55">
         <v>0.08</v>
@@ -15492,7 +16152,7 @@
         <v>140</v>
       </c>
       <c r="C56" t="s">
-        <v>400</v>
+        <v>502</v>
       </c>
       <c r="D56" t="s">
         <v>401</v>
@@ -15524,7 +16184,7 @@
         <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>402</v>
+        <v>503</v>
       </c>
       <c r="D57" t="s">
         <v>403</v>
@@ -15541,8 +16201,8 @@
       <c r="H57">
         <v>18.899999999999999</v>
       </c>
-      <c r="I57">
-        <v>680275060390</v>
+      <c r="I57" t="s">
+        <v>633</v>
       </c>
       <c r="J57">
         <v>0.23</v>
@@ -15556,7 +16216,7 @@
         <v>142</v>
       </c>
       <c r="C58" t="s">
-        <v>404</v>
+        <v>504</v>
       </c>
       <c r="D58" t="s">
         <v>405</v>
@@ -15573,8 +16233,8 @@
       <c r="H58">
         <v>18.899999999999999</v>
       </c>
-      <c r="I58">
-        <v>680275060406</v>
+      <c r="I58" t="s">
+        <v>634</v>
       </c>
       <c r="J58">
         <v>0.08</v>
@@ -15588,7 +16248,7 @@
         <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>429</v>
+        <v>505</v>
       </c>
       <c r="D59" t="s">
         <v>406</v>
@@ -15605,8 +16265,8 @@
       <c r="H59">
         <v>18.899999999999999</v>
       </c>
-      <c r="I59">
-        <v>680275060413</v>
+      <c r="I59" t="s">
+        <v>635</v>
       </c>
       <c r="J59">
         <v>0.23</v>
@@ -15620,7 +16280,7 @@
         <v>144</v>
       </c>
       <c r="C60" t="s">
-        <v>407</v>
+        <v>506</v>
       </c>
       <c r="D60" t="s">
         <v>408</v>
@@ -15629,7 +16289,7 @@
         <v>16</v>
       </c>
       <c r="F60" t="s">
-        <v>186</v>
+        <v>437</v>
       </c>
       <c r="G60">
         <v>10.57</v>
@@ -15637,8 +16297,8 @@
       <c r="H60">
         <v>18.899999999999999</v>
       </c>
-      <c r="I60">
-        <v>680275060437</v>
+      <c r="I60" t="s">
+        <v>636</v>
       </c>
       <c r="J60">
         <v>0.08</v>
@@ -15652,7 +16312,7 @@
         <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>409</v>
+        <v>507</v>
       </c>
       <c r="D61" t="s">
         <v>410</v>
@@ -15661,7 +16321,7 @@
         <v>16</v>
       </c>
       <c r="F61" t="s">
-        <v>186</v>
+        <v>437</v>
       </c>
       <c r="G61">
         <v>10.57</v>
@@ -15669,8 +16329,8 @@
       <c r="H61">
         <v>18.899999999999999</v>
       </c>
-      <c r="I61">
-        <v>680275060420</v>
+      <c r="I61" t="s">
+        <v>637</v>
       </c>
       <c r="J61">
         <v>0.08</v>
@@ -15684,7 +16344,7 @@
         <v>146</v>
       </c>
       <c r="C62" t="s">
-        <v>412</v>
+        <v>508</v>
       </c>
       <c r="D62" t="s">
         <v>411</v>
@@ -15693,7 +16353,7 @@
         <v>16</v>
       </c>
       <c r="F62" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G62">
         <v>10.57</v>
@@ -15701,8 +16361,8 @@
       <c r="H62">
         <v>18.899999999999999</v>
       </c>
-      <c r="I62">
-        <v>680275060444</v>
+      <c r="I62" t="s">
+        <v>638</v>
       </c>
       <c r="J62">
         <v>0.23</v>
@@ -15716,7 +16376,7 @@
         <v>147</v>
       </c>
       <c r="C63" t="s">
-        <v>413</v>
+        <v>509</v>
       </c>
       <c r="D63" t="s">
         <v>414</v>
@@ -15733,8 +16393,8 @@
       <c r="H63">
         <v>18.899999999999999</v>
       </c>
-      <c r="I63">
-        <v>680275060161</v>
+      <c r="I63" t="s">
+        <v>639</v>
       </c>
       <c r="J63">
         <v>0.08</v>
@@ -15748,7 +16408,7 @@
         <v>148</v>
       </c>
       <c r="C64" t="s">
-        <v>415</v>
+        <v>510</v>
       </c>
       <c r="D64" t="s">
         <v>416</v>
@@ -15765,8 +16425,8 @@
       <c r="H64">
         <v>18.899999999999999</v>
       </c>
-      <c r="I64">
-        <v>680275060178</v>
+      <c r="I64" t="s">
+        <v>640</v>
       </c>
       <c r="J64">
         <v>0.08</v>
@@ -15780,7 +16440,7 @@
         <v>149</v>
       </c>
       <c r="C65" t="s">
-        <v>430</v>
+        <v>511</v>
       </c>
       <c r="D65" t="s">
         <v>417</v>
@@ -15797,8 +16457,8 @@
       <c r="H65">
         <v>18.899999999999999</v>
       </c>
-      <c r="I65">
-        <v>680275060154</v>
+      <c r="I65" t="s">
+        <v>641</v>
       </c>
       <c r="J65">
         <v>0.08</v>
@@ -15812,7 +16472,7 @@
         <v>150</v>
       </c>
       <c r="C66" t="s">
-        <v>431</v>
+        <v>512</v>
       </c>
       <c r="D66" t="s">
         <v>418</v>
@@ -15829,8 +16489,8 @@
       <c r="H66">
         <v>18.899999999999999</v>
       </c>
-      <c r="I66">
-        <v>680275060185</v>
+      <c r="I66" t="s">
+        <v>642</v>
       </c>
       <c r="J66">
         <v>0.23</v>
@@ -15844,7 +16504,7 @@
         <v>168</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>513</v>
       </c>
       <c r="D67" t="s">
         <v>356</v>
@@ -15853,7 +16513,7 @@
         <v>159</v>
       </c>
       <c r="F67" t="s">
-        <v>188</v>
+        <v>438</v>
       </c>
       <c r="G67">
         <v>10.57</v>
@@ -15876,7 +16536,7 @@
         <v>169</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>514</v>
       </c>
       <c r="D68" t="s">
         <v>397</v>
@@ -15885,7 +16545,7 @@
         <v>159</v>
       </c>
       <c r="F68" t="s">
-        <v>189</v>
+        <v>439</v>
       </c>
       <c r="G68">
         <v>10.57</v>
@@ -15893,8 +16553,8 @@
       <c r="H68">
         <v>18.899999999999999</v>
       </c>
-      <c r="I68">
-        <v>680275059455</v>
+      <c r="I68" t="s">
+        <v>643</v>
       </c>
       <c r="J68">
         <v>0.23</v>
@@ -15908,7 +16568,7 @@
         <v>326</v>
       </c>
       <c r="C69" t="s">
-        <v>327</v>
+        <v>515</v>
       </c>
       <c r="D69" t="s">
         <v>376</v>
@@ -15917,7 +16577,7 @@
         <v>16</v>
       </c>
       <c r="F69" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G69">
         <v>10.57</v>
@@ -15925,8 +16585,8 @@
       <c r="H69">
         <v>18.899999999999999</v>
       </c>
-      <c r="I69">
-        <v>680275059615</v>
+      <c r="I69" t="s">
+        <v>644</v>
       </c>
       <c r="J69">
         <v>0.08</v>
@@ -15940,7 +16600,7 @@
         <v>170</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>516</v>
       </c>
       <c r="D70" t="s">
         <v>398</v>
@@ -15949,7 +16609,7 @@
         <v>16</v>
       </c>
       <c r="F70" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G70">
         <v>10.57</v>
@@ -15972,7 +16632,7 @@
         <v>171</v>
       </c>
       <c r="C71" t="s">
-        <v>155</v>
+        <v>517</v>
       </c>
       <c r="D71" t="s">
         <v>362</v>
@@ -15981,7 +16641,7 @@
         <v>159</v>
       </c>
       <c r="F71" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G71">
         <v>10.57</v>
@@ -15989,8 +16649,8 @@
       <c r="H71">
         <v>18.899999999999999</v>
       </c>
-      <c r="I71">
-        <v>680275059493</v>
+      <c r="I71" t="s">
+        <v>645</v>
       </c>
       <c r="J71">
         <v>0.23</v>
@@ -16004,7 +16664,7 @@
         <v>172</v>
       </c>
       <c r="C72" t="s">
-        <v>92</v>
+        <v>518</v>
       </c>
       <c r="D72" t="s">
         <v>358</v>
@@ -16013,7 +16673,7 @@
         <v>16</v>
       </c>
       <c r="F72" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G72">
         <v>10.57</v>
@@ -16021,8 +16681,8 @@
       <c r="H72">
         <v>18.899999999999999</v>
       </c>
-      <c r="I72">
-        <v>680275059509</v>
+      <c r="I72" t="s">
+        <v>646</v>
       </c>
       <c r="J72">
         <v>0.23</v>
@@ -16036,7 +16696,7 @@
         <v>173</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>519</v>
       </c>
       <c r="D73" t="s">
         <v>399</v>
@@ -16045,7 +16705,7 @@
         <v>159</v>
       </c>
       <c r="F73" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G73">
         <v>10.57</v>
@@ -16053,8 +16713,8 @@
       <c r="H73">
         <v>18.899999999999999</v>
       </c>
-      <c r="I73">
-        <v>680275059516</v>
+      <c r="I73" t="s">
+        <v>647</v>
       </c>
       <c r="J73">
         <v>0.23</v>
@@ -16068,13 +16728,13 @@
         <v>174</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>520</v>
       </c>
       <c r="E74" t="s">
         <v>16</v>
       </c>
       <c r="F74" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G74">
         <v>10.57</v>
@@ -16082,8 +16742,8 @@
       <c r="H74">
         <v>18.899999999999999</v>
       </c>
-      <c r="I74">
-        <v>680275059523</v>
+      <c r="I74" t="s">
+        <v>648</v>
       </c>
       <c r="J74">
         <v>0.23</v>
@@ -16097,13 +16757,13 @@
         <v>175</v>
       </c>
       <c r="C75" t="s">
-        <v>36</v>
+        <v>521</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
       </c>
       <c r="F75" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G75">
         <v>10.57</v>
@@ -16111,8 +16771,8 @@
       <c r="H75">
         <v>18.899999999999999</v>
       </c>
-      <c r="I75">
-        <v>680275059530</v>
+      <c r="I75" t="s">
+        <v>649</v>
       </c>
       <c r="J75">
         <v>0.23</v>
@@ -16126,13 +16786,13 @@
         <v>176</v>
       </c>
       <c r="C76" t="s">
-        <v>157</v>
+        <v>522</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
       </c>
       <c r="F76" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G76">
         <v>10.57</v>
@@ -16140,8 +16800,8 @@
       <c r="H76">
         <v>18.899999999999999</v>
       </c>
-      <c r="I76">
-        <v>680275059578</v>
+      <c r="I76" t="s">
+        <v>650</v>
       </c>
       <c r="J76">
         <v>0.23</v>
@@ -16155,13 +16815,13 @@
         <v>177</v>
       </c>
       <c r="C77" t="s">
-        <v>44</v>
+        <v>523</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
       </c>
       <c r="F77" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G77">
         <v>10.57</v>
@@ -16169,8 +16829,8 @@
       <c r="H77">
         <v>18.899999999999999</v>
       </c>
-      <c r="I77">
-        <v>680275059585</v>
+      <c r="I77" t="s">
+        <v>651</v>
       </c>
       <c r="J77">
         <v>0.08</v>
@@ -16184,13 +16844,13 @@
         <v>178</v>
       </c>
       <c r="C78" t="s">
-        <v>65</v>
+        <v>524</v>
       </c>
       <c r="E78" t="s">
         <v>16</v>
       </c>
       <c r="F78" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G78">
         <v>10.57</v>
@@ -16198,8 +16858,8 @@
       <c r="H78">
         <v>18.899999999999999</v>
       </c>
-      <c r="I78">
-        <v>680275059622</v>
+      <c r="I78" t="s">
+        <v>652</v>
       </c>
       <c r="J78">
         <v>0.08</v>
@@ -16213,13 +16873,13 @@
         <v>178</v>
       </c>
       <c r="C79" t="s">
-        <v>158</v>
+        <v>525</v>
       </c>
       <c r="E79" t="s">
         <v>16</v>
       </c>
       <c r="F79" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G79">
         <v>10.57</v>
@@ -16227,8 +16887,8 @@
       <c r="H79">
         <v>18.899999999999999</v>
       </c>
-      <c r="I79">
-        <v>680275059660</v>
+      <c r="I79" t="s">
+        <v>653</v>
       </c>
       <c r="J79">
         <v>0.08</v>
@@ -16242,13 +16902,13 @@
         <v>179</v>
       </c>
       <c r="C80" t="s">
-        <v>69</v>
+        <v>526</v>
       </c>
       <c r="E80" t="s">
         <v>16</v>
       </c>
       <c r="F80" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G80">
         <v>10.57</v>
@@ -16256,8 +16916,8 @@
       <c r="H80">
         <v>18.899999999999999</v>
       </c>
-      <c r="I80">
-        <v>680275059677</v>
+      <c r="I80" t="s">
+        <v>654</v>
       </c>
       <c r="J80">
         <v>0.08</v>
@@ -16271,13 +16931,13 @@
         <v>180</v>
       </c>
       <c r="C81" t="s">
-        <v>85</v>
+        <v>527</v>
       </c>
       <c r="E81" t="s">
         <v>16</v>
       </c>
       <c r="F81" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G81">
         <v>10.57</v>
@@ -16285,8 +16945,8 @@
       <c r="H81">
         <v>18.899999999999999</v>
       </c>
-      <c r="I81">
-        <v>680275059707</v>
+      <c r="I81" t="s">
+        <v>655</v>
       </c>
       <c r="J81">
         <v>0.08</v>
@@ -16300,13 +16960,13 @@
         <v>181</v>
       </c>
       <c r="C82" t="s">
-        <v>75</v>
+        <v>528</v>
       </c>
       <c r="E82" t="s">
         <v>16</v>
       </c>
       <c r="F82" t="s">
-        <v>160</v>
+        <v>440</v>
       </c>
       <c r="G82">
         <v>10.57</v>
@@ -16314,8 +16974,8 @@
       <c r="H82">
         <v>18.899999999999999</v>
       </c>
-      <c r="I82">
-        <v>680275059721</v>
+      <c r="I82" t="s">
+        <v>656</v>
       </c>
       <c r="J82">
         <v>0.08</v>
@@ -16329,7 +16989,7 @@
         <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>432</v>
+        <v>529</v>
       </c>
       <c r="E83" t="s">
         <v>159</v>
@@ -16358,7 +17018,7 @@
         <v>222</v>
       </c>
       <c r="C84" t="s">
-        <v>433</v>
+        <v>530</v>
       </c>
       <c r="E84" t="s">
         <v>16</v>
@@ -16387,7 +17047,7 @@
         <v>223</v>
       </c>
       <c r="C85" t="s">
-        <v>434</v>
+        <v>531</v>
       </c>
       <c r="E85" t="s">
         <v>159</v>
@@ -16416,7 +17076,7 @@
         <v>224</v>
       </c>
       <c r="C86" t="s">
-        <v>435</v>
+        <v>532</v>
       </c>
       <c r="E86" t="s">
         <v>159</v>
@@ -16445,7 +17105,7 @@
         <v>225</v>
       </c>
       <c r="C87" t="s">
-        <v>436</v>
+        <v>533</v>
       </c>
       <c r="E87" t="s">
         <v>159</v>
@@ -16474,7 +17134,7 @@
         <v>226</v>
       </c>
       <c r="C88" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="E88" t="s">
         <v>16</v>
@@ -16503,7 +17163,7 @@
         <v>227</v>
       </c>
       <c r="C89" t="s">
-        <v>438</v>
+        <v>535</v>
       </c>
       <c r="E89" t="s">
         <v>16</v>
@@ -16532,7 +17192,7 @@
         <v>228</v>
       </c>
       <c r="C90" t="s">
-        <v>439</v>
+        <v>536</v>
       </c>
       <c r="D90" t="s">
         <v>343</v>
@@ -16564,7 +17224,7 @@
         <v>229</v>
       </c>
       <c r="C91" t="s">
-        <v>440</v>
+        <v>537</v>
       </c>
       <c r="D91" t="s">
         <v>342</v>
@@ -16596,7 +17256,7 @@
         <v>230</v>
       </c>
       <c r="C92" t="s">
-        <v>240</v>
+        <v>538</v>
       </c>
       <c r="D92" t="s">
         <v>344</v>
@@ -16628,13 +17288,13 @@
         <v>248</v>
       </c>
       <c r="C93" t="s">
-        <v>441</v>
+        <v>539</v>
       </c>
       <c r="E93" t="s">
         <v>159</v>
       </c>
       <c r="F93" t="s">
-        <v>260</v>
+        <v>441</v>
       </c>
       <c r="G93">
         <v>40.65</v>
@@ -16657,13 +17317,13 @@
         <v>249</v>
       </c>
       <c r="C94" t="s">
-        <v>442</v>
+        <v>540</v>
       </c>
       <c r="E94" t="s">
         <v>159</v>
       </c>
       <c r="F94" t="s">
-        <v>261</v>
+        <v>442</v>
       </c>
       <c r="G94">
         <v>40.65</v>
@@ -16686,13 +17346,13 @@
         <v>250</v>
       </c>
       <c r="C95" t="s">
-        <v>443</v>
+        <v>541</v>
       </c>
       <c r="E95" t="s">
         <v>159</v>
       </c>
       <c r="F95" t="s">
-        <v>262</v>
+        <v>443</v>
       </c>
       <c r="G95">
         <v>40.65</v>
@@ -16715,13 +17375,13 @@
         <v>251</v>
       </c>
       <c r="C96" t="s">
-        <v>444</v>
+        <v>542</v>
       </c>
       <c r="E96" t="s">
         <v>16</v>
       </c>
       <c r="F96" t="s">
-        <v>262</v>
+        <v>443</v>
       </c>
       <c r="G96">
         <v>40.65</v>
@@ -16744,13 +17404,13 @@
         <v>252</v>
       </c>
       <c r="C97" t="s">
-        <v>445</v>
+        <v>543</v>
       </c>
       <c r="E97" t="s">
         <v>16</v>
       </c>
       <c r="F97" t="s">
-        <v>262</v>
+        <v>443</v>
       </c>
       <c r="G97">
         <v>40.65</v>
@@ -16773,13 +17433,13 @@
         <v>253</v>
       </c>
       <c r="C98" t="s">
-        <v>446</v>
+        <v>544</v>
       </c>
       <c r="E98" t="s">
         <v>159</v>
       </c>
       <c r="F98" t="s">
-        <v>262</v>
+        <v>443</v>
       </c>
       <c r="G98">
         <v>40.65</v>
@@ -16802,13 +17462,13 @@
         <v>202</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>545</v>
       </c>
       <c r="E99" t="s">
         <v>159</v>
       </c>
       <c r="F99" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G99">
         <v>21.06</v>
@@ -16816,8 +17476,8 @@
       <c r="H99">
         <v>36.9</v>
       </c>
-      <c r="I99">
-        <v>680275060055</v>
+      <c r="I99" t="s">
+        <v>657</v>
       </c>
       <c r="J99">
         <v>0.23</v>
@@ -16831,13 +17491,13 @@
         <v>192</v>
       </c>
       <c r="C100" t="s">
-        <v>161</v>
+        <v>546</v>
       </c>
       <c r="E100" t="s">
         <v>16</v>
       </c>
       <c r="F100" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G100">
         <v>21.06</v>
@@ -16845,8 +17505,8 @@
       <c r="H100">
         <v>36.9</v>
       </c>
-      <c r="I100">
-        <v>680275059820</v>
+      <c r="I100" t="s">
+        <v>658</v>
       </c>
       <c r="J100">
         <v>0.23</v>
@@ -16860,13 +17520,13 @@
         <v>199</v>
       </c>
       <c r="C101" t="s">
-        <v>162</v>
+        <v>547</v>
       </c>
       <c r="E101" t="s">
         <v>16</v>
       </c>
       <c r="F101" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G101">
         <v>21.06</v>
@@ -16874,8 +17534,8 @@
       <c r="H101">
         <v>36.9</v>
       </c>
-      <c r="I101">
-        <v>680275059844</v>
+      <c r="I101" t="s">
+        <v>659</v>
       </c>
       <c r="J101">
         <v>0.23</v>
@@ -16889,13 +17549,13 @@
         <v>204</v>
       </c>
       <c r="C102" t="s">
-        <v>163</v>
+        <v>548</v>
       </c>
       <c r="E102" t="s">
         <v>16</v>
       </c>
       <c r="F102" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G102">
         <v>21.06</v>
@@ -16903,8 +17563,8 @@
       <c r="H102">
         <v>36.9</v>
       </c>
-      <c r="I102">
-        <v>680275059868</v>
+      <c r="I102" t="s">
+        <v>660</v>
       </c>
       <c r="J102">
         <v>0.23</v>
@@ -16918,13 +17578,13 @@
         <v>197</v>
       </c>
       <c r="C103" t="s">
-        <v>92</v>
+        <v>549</v>
       </c>
       <c r="E103" t="s">
         <v>16</v>
       </c>
       <c r="F103" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G103">
         <v>21.06</v>
@@ -16932,8 +17592,8 @@
       <c r="H103">
         <v>36.9</v>
       </c>
-      <c r="I103">
-        <v>680275059889</v>
+      <c r="I103" t="s">
+        <v>661</v>
       </c>
       <c r="J103">
         <v>0.23</v>
@@ -16947,13 +17607,13 @@
         <v>194</v>
       </c>
       <c r="C104" t="s">
-        <v>164</v>
+        <v>550</v>
       </c>
       <c r="E104" t="s">
         <v>159</v>
       </c>
       <c r="F104" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G104">
         <v>21.06</v>
@@ -16961,8 +17621,8 @@
       <c r="H104">
         <v>36.9</v>
       </c>
-      <c r="I104">
-        <v>680275059912</v>
+      <c r="I104" t="s">
+        <v>662</v>
       </c>
       <c r="J104">
         <v>0.23</v>
@@ -16976,13 +17636,13 @@
         <v>190</v>
       </c>
       <c r="C105" t="s">
-        <v>94</v>
+        <v>551</v>
       </c>
       <c r="E105" t="s">
         <v>16</v>
       </c>
       <c r="F105" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G105">
         <v>21.06</v>
@@ -16990,8 +17650,8 @@
       <c r="H105">
         <v>36.9</v>
       </c>
-      <c r="I105">
-        <v>680275059929</v>
+      <c r="I105" t="s">
+        <v>663</v>
       </c>
       <c r="J105">
         <v>0.23</v>
@@ -17005,13 +17665,13 @@
         <v>203</v>
       </c>
       <c r="C106" t="s">
-        <v>36</v>
+        <v>552</v>
       </c>
       <c r="E106" t="s">
         <v>16</v>
       </c>
       <c r="F106" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G106">
         <v>21.06</v>
@@ -17019,8 +17679,8 @@
       <c r="H106">
         <v>36.9</v>
       </c>
-      <c r="I106">
-        <v>680275059936</v>
+      <c r="I106" t="s">
+        <v>664</v>
       </c>
       <c r="J106">
         <v>0.23</v>
@@ -17034,13 +17694,13 @@
         <v>191</v>
       </c>
       <c r="C107" t="s">
-        <v>99</v>
+        <v>553</v>
       </c>
       <c r="E107" t="s">
         <v>159</v>
       </c>
       <c r="F107" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G107">
         <v>21.06</v>
@@ -17048,8 +17708,8 @@
       <c r="H107">
         <v>36.9</v>
       </c>
-      <c r="I107">
-        <v>680275059967</v>
+      <c r="I107" t="s">
+        <v>665</v>
       </c>
       <c r="J107">
         <v>0.08</v>
@@ -17063,13 +17723,13 @@
         <v>329</v>
       </c>
       <c r="C108" t="s">
-        <v>38</v>
+        <v>554</v>
       </c>
       <c r="E108" t="s">
         <v>16</v>
       </c>
       <c r="F108" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G108">
         <v>21.06</v>
@@ -17077,8 +17737,8 @@
       <c r="H108">
         <v>36.9</v>
       </c>
-      <c r="I108">
-        <v>680275059974</v>
+      <c r="I108" t="s">
+        <v>666</v>
       </c>
       <c r="J108">
         <v>0.23</v>
@@ -17092,13 +17752,13 @@
         <v>193</v>
       </c>
       <c r="C109" t="s">
-        <v>102</v>
+        <v>555</v>
       </c>
       <c r="E109" t="s">
         <v>159</v>
       </c>
       <c r="F109" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G109">
         <v>21.06</v>
@@ -17106,8 +17766,8 @@
       <c r="H109">
         <v>36.9</v>
       </c>
-      <c r="I109">
-        <v>680275059998</v>
+      <c r="I109" t="s">
+        <v>667</v>
       </c>
       <c r="J109">
         <v>0.08</v>
@@ -17121,13 +17781,13 @@
         <v>205</v>
       </c>
       <c r="C110" t="s">
-        <v>165</v>
+        <v>556</v>
       </c>
       <c r="E110" t="s">
         <v>16</v>
       </c>
       <c r="F110" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G110">
         <v>21.06</v>
@@ -17135,8 +17795,8 @@
       <c r="H110">
         <v>36.9</v>
       </c>
-      <c r="I110">
-        <v>680275060000</v>
+      <c r="I110" t="s">
+        <v>668</v>
       </c>
       <c r="J110">
         <v>0.23</v>
@@ -17150,13 +17810,13 @@
         <v>330</v>
       </c>
       <c r="C111" t="s">
-        <v>51</v>
+        <v>557</v>
       </c>
       <c r="E111" t="s">
         <v>16</v>
       </c>
       <c r="F111" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G111">
         <v>21.06</v>
@@ -17164,8 +17824,8 @@
       <c r="H111">
         <v>36.9</v>
       </c>
-      <c r="I111">
-        <v>680275060024</v>
+      <c r="I111" t="s">
+        <v>669</v>
       </c>
       <c r="J111">
         <v>0.08</v>
@@ -17179,13 +17839,13 @@
         <v>195</v>
       </c>
       <c r="C112" t="s">
-        <v>166</v>
+        <v>558</v>
       </c>
       <c r="E112" t="s">
         <v>16</v>
       </c>
       <c r="F112" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G112">
         <v>21.06</v>
@@ -17193,8 +17853,8 @@
       <c r="H112">
         <v>36.9</v>
       </c>
-      <c r="I112">
-        <v>680275060048</v>
+      <c r="I112" t="s">
+        <v>670</v>
       </c>
       <c r="J112">
         <v>0.08</v>
@@ -17208,13 +17868,13 @@
         <v>196</v>
       </c>
       <c r="C113" t="s">
-        <v>155</v>
+        <v>559</v>
       </c>
       <c r="E113" t="s">
         <v>159</v>
       </c>
       <c r="F113" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G113">
         <v>21.06</v>
@@ -17222,8 +17882,8 @@
       <c r="H113">
         <v>36.9</v>
       </c>
-      <c r="I113">
-        <v>680275059882</v>
+      <c r="I113" t="s">
+        <v>671</v>
       </c>
       <c r="J113">
         <v>0.23</v>
@@ -17237,13 +17897,13 @@
         <v>201</v>
       </c>
       <c r="C114" t="s">
-        <v>154</v>
+        <v>560</v>
       </c>
       <c r="E114" t="s">
         <v>159</v>
       </c>
       <c r="F114" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G114">
         <v>24.31</v>
@@ -17251,8 +17911,8 @@
       <c r="H114">
         <v>36.9</v>
       </c>
-      <c r="I114">
-        <v>680275059813</v>
+      <c r="I114" t="s">
+        <v>672</v>
       </c>
       <c r="J114">
         <v>0.23</v>
@@ -17266,13 +17926,13 @@
         <v>200</v>
       </c>
       <c r="C115" t="s">
-        <v>44</v>
+        <v>561</v>
       </c>
       <c r="E115" t="s">
         <v>16</v>
       </c>
       <c r="F115" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G115">
         <v>21.06</v>
@@ -17280,8 +17940,8 @@
       <c r="H115">
         <v>36.9</v>
       </c>
-      <c r="I115">
-        <v>680275060017</v>
+      <c r="I115" t="s">
+        <v>673</v>
       </c>
       <c r="J115">
         <v>0.08</v>
@@ -17295,13 +17955,13 @@
         <v>198</v>
       </c>
       <c r="C116" t="s">
-        <v>69</v>
+        <v>562</v>
       </c>
       <c r="E116" t="s">
         <v>16</v>
       </c>
       <c r="F116" t="s">
-        <v>167</v>
+        <v>444</v>
       </c>
       <c r="G116">
         <v>21.06</v>
@@ -17309,8 +17969,8 @@
       <c r="H116">
         <v>36.9</v>
       </c>
-      <c r="I116">
-        <v>680275059806</v>
+      <c r="I116" t="s">
+        <v>674</v>
       </c>
       <c r="J116">
         <v>0.08</v>
@@ -17324,7 +17984,7 @@
         <v>312</v>
       </c>
       <c r="C117" t="s">
-        <v>447</v>
+        <v>563</v>
       </c>
       <c r="D117" t="s">
         <v>356</v>
@@ -17333,7 +17993,7 @@
         <v>159</v>
       </c>
       <c r="F117" t="s">
-        <v>318</v>
+        <v>445</v>
       </c>
       <c r="G117">
         <v>18.600000000000001</v>
@@ -17356,7 +18016,7 @@
         <v>314</v>
       </c>
       <c r="C118" t="s">
-        <v>448</v>
+        <v>564</v>
       </c>
       <c r="D118" t="s">
         <v>389</v>
@@ -17365,7 +18025,7 @@
         <v>159</v>
       </c>
       <c r="F118" t="s">
-        <v>317</v>
+        <v>446</v>
       </c>
       <c r="G118">
         <v>18.600000000000001</v>
@@ -17388,7 +18048,7 @@
         <v>297</v>
       </c>
       <c r="C119" t="s">
-        <v>449</v>
+        <v>565</v>
       </c>
       <c r="D119" t="s">
         <v>390</v>
@@ -17397,7 +18057,7 @@
         <v>16</v>
       </c>
       <c r="F119" t="s">
-        <v>316</v>
+        <v>447</v>
       </c>
       <c r="G119">
         <v>17.8</v>
@@ -17405,8 +18065,8 @@
       <c r="H119">
         <v>31.9</v>
       </c>
-      <c r="I119">
-        <v>680275060864</v>
+      <c r="I119" t="s">
+        <v>675</v>
       </c>
       <c r="J119">
         <v>0.23</v>
@@ -17420,7 +18080,7 @@
         <v>299</v>
       </c>
       <c r="C120" t="s">
-        <v>450</v>
+        <v>566</v>
       </c>
       <c r="D120" t="s">
         <v>391</v>
@@ -17429,7 +18089,7 @@
         <v>16</v>
       </c>
       <c r="F120" t="s">
-        <v>316</v>
+        <v>447</v>
       </c>
       <c r="G120">
         <v>17.8</v>
@@ -17437,8 +18097,8 @@
       <c r="H120">
         <v>31.9</v>
       </c>
-      <c r="I120">
-        <v>680275060871</v>
+      <c r="I120" t="s">
+        <v>676</v>
       </c>
       <c r="J120">
         <v>0.08</v>
@@ -17452,7 +18112,7 @@
         <v>301</v>
       </c>
       <c r="C121" t="s">
-        <v>451</v>
+        <v>567</v>
       </c>
       <c r="D121" t="s">
         <v>392</v>
@@ -17461,7 +18121,7 @@
         <v>16</v>
       </c>
       <c r="F121" t="s">
-        <v>316</v>
+        <v>447</v>
       </c>
       <c r="G121">
         <v>17.8</v>
@@ -17469,8 +18129,8 @@
       <c r="H121">
         <v>31.9</v>
       </c>
-      <c r="I121">
-        <v>680275060888</v>
+      <c r="I121" t="s">
+        <v>677</v>
       </c>
       <c r="J121">
         <v>0.08</v>
@@ -17484,7 +18144,7 @@
         <v>282</v>
       </c>
       <c r="C122" t="s">
-        <v>452</v>
+        <v>568</v>
       </c>
       <c r="D122" t="s">
         <v>393</v>
@@ -17493,7 +18153,7 @@
         <v>16</v>
       </c>
       <c r="F122" t="s">
-        <v>316</v>
+        <v>447</v>
       </c>
       <c r="G122">
         <v>21.06</v>
@@ -17516,7 +18176,7 @@
         <v>295</v>
       </c>
       <c r="C123" t="s">
-        <v>453</v>
+        <v>569</v>
       </c>
       <c r="D123" t="s">
         <v>394</v>
@@ -17533,8 +18193,8 @@
       <c r="H123">
         <v>46.9</v>
       </c>
-      <c r="I123">
-        <v>680275060857</v>
+      <c r="I123" t="s">
+        <v>678</v>
       </c>
       <c r="J123">
         <v>0.23</v>
@@ -17548,7 +18208,7 @@
         <v>303</v>
       </c>
       <c r="C124" t="s">
-        <v>454</v>
+        <v>570</v>
       </c>
       <c r="D124" t="s">
         <v>381</v>
@@ -17580,7 +18240,7 @@
         <v>288</v>
       </c>
       <c r="C125" t="s">
-        <v>455</v>
+        <v>571</v>
       </c>
       <c r="D125" t="s">
         <v>396</v>
@@ -17612,7 +18272,7 @@
         <v>265</v>
       </c>
       <c r="C126" t="s">
-        <v>456</v>
+        <v>572</v>
       </c>
       <c r="D126" t="s">
         <v>381</v>
@@ -17644,7 +18304,7 @@
         <v>263</v>
       </c>
       <c r="C127" t="s">
-        <v>457</v>
+        <v>573</v>
       </c>
       <c r="D127" t="s">
         <v>380</v>
@@ -17676,7 +18336,7 @@
         <v>264</v>
       </c>
       <c r="C128" t="s">
-        <v>458</v>
+        <v>574</v>
       </c>
       <c r="D128" t="s">
         <v>379</v>
@@ -17708,7 +18368,7 @@
         <v>266</v>
       </c>
       <c r="C129" t="s">
-        <v>459</v>
+        <v>575</v>
       </c>
       <c r="D129" t="s">
         <v>382</v>
@@ -17725,8 +18385,8 @@
       <c r="H129">
         <v>52.9</v>
       </c>
-      <c r="I129">
-        <v>680275060826</v>
+      <c r="I129" t="s">
+        <v>679</v>
       </c>
       <c r="J129">
         <v>0.23</v>
@@ -17740,7 +18400,7 @@
         <v>308</v>
       </c>
       <c r="C130" t="s">
-        <v>460</v>
+        <v>576</v>
       </c>
       <c r="D130" t="s">
         <v>384</v>
@@ -17757,8 +18417,8 @@
       <c r="H130">
         <v>78.900000000000006</v>
       </c>
-      <c r="I130">
-        <v>680275058175</v>
+      <c r="I130" t="s">
+        <v>680</v>
       </c>
       <c r="J130">
         <v>0.08</v>
@@ -17772,7 +18432,7 @@
         <v>305</v>
       </c>
       <c r="C131" t="s">
-        <v>461</v>
+        <v>577</v>
       </c>
       <c r="D131" t="s">
         <v>383</v>
@@ -17789,8 +18449,8 @@
       <c r="H131">
         <v>78.900000000000006</v>
       </c>
-      <c r="I131">
-        <v>680275060833</v>
+      <c r="I131" t="s">
+        <v>681</v>
       </c>
       <c r="J131">
         <v>0.23</v>
@@ -17804,7 +18464,7 @@
         <v>307</v>
       </c>
       <c r="C132" t="s">
-        <v>462</v>
+        <v>578</v>
       </c>
       <c r="D132" t="s">
         <v>383</v>
@@ -17821,8 +18481,8 @@
       <c r="H132">
         <v>78.900000000000006</v>
       </c>
-      <c r="I132">
-        <v>680275060840</v>
+      <c r="I132" t="s">
+        <v>682</v>
       </c>
       <c r="J132">
         <v>0.23</v>

</xml_diff>